<commit_message>
Team Attendance[B8-B1] 02 Aug 23
Team Attendance[B8-B1] 02 Aug 23
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CODE-MIND\Angular\JS-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A6D250B-8285-4307-840A-529DD20C8D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC66BE6-5352-42A7-BF08-731B01A41BCA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -132,7 +132,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -143,9 +143,6 @@
     <t>PRESENT</t>
   </si>
   <si>
-    <t>Niketan Thombare(TL)</t>
-  </si>
-  <si>
     <t>Vinay Madne</t>
   </si>
   <si>
@@ -155,29 +152,32 @@
     <t>Sanket Chaudhari</t>
   </si>
   <si>
-    <t>Vishwajeet Jamdade</t>
-  </si>
-  <si>
     <t>Kishor Ubhale</t>
   </si>
   <si>
     <t>Sachin hake</t>
   </si>
   <si>
-    <t>Ashutosh Wakde</t>
-  </si>
-  <si>
-    <t>Uday Wankhede</t>
-  </si>
-  <si>
-    <t>RaviK Suryawanshi</t>
+    <t>Niketan (TL)</t>
+  </si>
+  <si>
+    <t>Vishwajeet J</t>
+  </si>
+  <si>
+    <t>Ashutosh W</t>
+  </si>
+  <si>
+    <t>Uday W</t>
+  </si>
+  <si>
+    <t>RaviKumar S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -206,13 +206,25 @@
       <name val="Tahoma"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -227,7 +239,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -238,6 +250,8 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -554,48 +568,50 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
   <dimension ref="A1:L3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H7" sqref="H7"/>
+      <selection pane="bottomLeft" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.5" customWidth="1"/>
-    <col min="2" max="2" width="19.5" customWidth="1"/>
+    <col min="2" max="2" width="14.75" customWidth="1"/>
     <col min="3" max="3" width="14.125" customWidth="1"/>
     <col min="4" max="4" width="14.375" customWidth="1"/>
     <col min="5" max="5" width="18.75" customWidth="1"/>
-    <col min="6" max="6" width="16.25" customWidth="1"/>
-    <col min="7" max="7" width="14.25" customWidth="1"/>
+    <col min="6" max="6" width="14" customWidth="1"/>
+    <col min="7" max="7" width="14.875" customWidth="1"/>
     <col min="8" max="8" width="12.625" customWidth="1"/>
-    <col min="9" max="9" width="14.5" customWidth="1"/>
+    <col min="9" max="9" width="13" customWidth="1"/>
+    <col min="10" max="10" width="12.75" customWidth="1"/>
+    <col min="11" max="11" width="15.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="3" customFormat="1" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>9</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>10</v>
@@ -612,7 +628,7 @@
       <c r="A2" s="5">
         <v>45140</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
       <c r="C2" t="s">
@@ -645,9 +661,6 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1"/>
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
     </row>
   </sheetData>
   <dataConsolidate/>
@@ -658,6 +671,7 @@
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Team Attendance B8-B1 - 10-Aug-23
Team Attendance B8-B1 - 10-Aug-23
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CODE-MIND\Angular\JS-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BE4CDE8-C01F-4182-AC51-2350C37E123C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42823061-42D3-40E1-9BB8-3A4E06631FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -487,12 +487,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="K9" authorId="0" shapeId="0" xr:uid="{EADACEC7-3B7F-4301-A9D1-D26DCF524639}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Document work</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -939,11 +963,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L8"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K8" sqref="K8"/>
+      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1242,6 +1266,41 @@
         <v>2</v>
       </c>
     </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="4">
+        <v>45148</v>
+      </c>
+      <c r="B9" t="s">
+        <v>2</v>
+      </c>
+      <c r="C9" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" t="s">
+        <v>2</v>
+      </c>
+      <c r="F9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9" t="s">
+        <v>2</v>
+      </c>
+      <c r="I9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J9" t="s">
+        <v>2</v>
+      </c>
+      <c r="K9" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Team Attendance 11-12 Aug 23
Team Attendance 11-12 Aug 23
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CODE-MIND\Angular\JS-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42823061-42D3-40E1-9BB8-3A4E06631FE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FC16CC7A-2DFC-49C4-811F-CC0EDB81B46B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -511,12 +511,301 @@
         </r>
       </text>
     </comment>
+    <comment ref="B10" authorId="0" shapeId="0" xr:uid="{1B9DA885-AB5D-48B1-9BD6-2A2ADA236A47}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Medical issue</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G10" authorId="0" shapeId="0" xr:uid="{E49AF9AC-6954-40C2-B0D1-F8ADE68BB1B3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Responsse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H10" authorId="0" shapeId="0" xr:uid="{E30E622B-4660-47AE-A6C3-582588955B15}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Responsse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I10" authorId="0" shapeId="0" xr:uid="{249F92BE-3B17-4CFF-948B-C68CEFAA8D03}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Responsse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J10" authorId="0" shapeId="0" xr:uid="{40000D96-B907-418A-BA3E-29817C5A5913}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Responsse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K10" authorId="0" shapeId="0" xr:uid="{D37402DB-B071-473F-8E5F-230E1494E59B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Responsse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{2D07EABC-2133-4FFC-A60B-B2F5EE7217C4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Medical issue</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{0BDE3FE7-14E0-47AF-83EC-88791B75CF52}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Responsse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{148A785A-3E70-499E-9AD9-46827764E520}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Responsse
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{0A571FDF-C559-4D94-AF76-076CE53023F4}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Responsse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J11" authorId="0" shapeId="0" xr:uid="{8B0FBD34-1A2F-4069-80BF-9959EC257983}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Responsse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K11" authorId="0" shapeId="0" xr:uid="{01472C97-1030-42B9-A66C-6EC38ED4BD49}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Responsse</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -963,11 +1252,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9"/>
+      <selection pane="bottomLeft" activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1301,6 +1590,79 @@
         <v>1</v>
       </c>
     </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="4">
+        <v>45149</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+      <c r="C10" t="s">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F10" t="s">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1</v>
+      </c>
+      <c r="H10" t="s">
+        <v>1</v>
+      </c>
+      <c r="I10" t="s">
+        <v>1</v>
+      </c>
+      <c r="J10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="4">
+        <v>45150</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+      <c r="C11" t="s">
+        <v>2</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" t="s">
+        <v>2</v>
+      </c>
+      <c r="F11" t="s">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>1</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1</v>
+      </c>
+      <c r="I11" t="s">
+        <v>1</v>
+      </c>
+      <c r="J11" t="s">
+        <v>1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
todays Team Attendance B8:B1 : 23-Aug-23
todays Team Attendance B8:B1 : 23-Aug-23
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CODE-MIND\Angular\JS-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17B8D4E7-C8F4-4060-8D2D-E34FB572329F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA32235-9A5C-4AF3-94A7-D72DA5C33BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1185,12 +1185,157 @@
         </r>
       </text>
     </comment>
+    <comment ref="D23" authorId="0" shapeId="0" xr:uid="{96B9E39E-890B-4D2C-BC4E-4A1D9768D857}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+outside
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G23" authorId="0" shapeId="0" xr:uid="{B0AD8011-51FB-44D4-B8C7-6CD848F53E4D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Headeche</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H23" authorId="0" shapeId="0" xr:uid="{CA3C3DCB-2DC1-4AD7-A8F0-6EE781F2969A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I23" authorId="0" shapeId="0" xr:uid="{13F57337-4FA0-433E-878F-973804C3966D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J23" authorId="0" shapeId="0" xr:uid="{8DAEAAD4-1D78-4AFA-BE58-34CB62345F98}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K23" authorId="0" shapeId="0" xr:uid="{65083A19-CBEE-4842-915E-68B23779357D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+having some work</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -1637,11 +1782,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L21"/>
+  <dimension ref="A1:L23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K21" sqref="K21"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2185,6 +2330,76 @@
         <v>2</v>
       </c>
     </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A22" s="4">
+        <v>45160</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>2</v>
+      </c>
+      <c r="D22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E22" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22" t="s">
+        <v>2</v>
+      </c>
+      <c r="I22" t="s">
+        <v>2</v>
+      </c>
+      <c r="J22" t="s">
+        <v>2</v>
+      </c>
+      <c r="K22" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A23" s="4">
+        <v>45161</v>
+      </c>
+      <c r="B23" t="s">
+        <v>2</v>
+      </c>
+      <c r="C23" t="s">
+        <v>2</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23" t="s">
+        <v>2</v>
+      </c>
+      <c r="F23" t="s">
+        <v>2</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1</v>
+      </c>
+      <c r="H23" t="s">
+        <v>1</v>
+      </c>
+      <c r="I23" t="s">
+        <v>1</v>
+      </c>
+      <c r="J23" t="s">
+        <v>1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Team Attendance B8B1 25_aug-23
Team Attendance B8B1 25_aug-23
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CODE-MIND\Angular\JS-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DA32235-9A5C-4AF3-94A7-D72DA5C33BF2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C245A5-B75E-4B8E-B432-F9F51A168609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1330,12 +1330,84 @@
         </r>
       </text>
     </comment>
+    <comment ref="J24" authorId="0" shapeId="0" xr:uid="{8431ED07-5B40-4F78-A141-F37031419457}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G25" authorId="0" shapeId="0" xr:uid="{6EFD5CD4-4C9E-44F4-8060-7EC9E2F7F155}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J25" authorId="0" shapeId="0" xr:uid="{4936ADF3-9109-4209-99FC-56DCC92E42C5}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -1782,11 +1854,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L23"/>
+  <dimension ref="A1:L25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G28" sqref="G28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2400,6 +2472,76 @@
         <v>1</v>
       </c>
     </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A24" s="4">
+        <v>45162</v>
+      </c>
+      <c r="B24" t="s">
+        <v>2</v>
+      </c>
+      <c r="C24" t="s">
+        <v>2</v>
+      </c>
+      <c r="D24" t="s">
+        <v>2</v>
+      </c>
+      <c r="E24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24" t="s">
+        <v>2</v>
+      </c>
+      <c r="I24" t="s">
+        <v>2</v>
+      </c>
+      <c r="J24" t="s">
+        <v>1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A25" s="4">
+        <v>45163</v>
+      </c>
+      <c r="B25" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" t="s">
+        <v>2</v>
+      </c>
+      <c r="D25" t="s">
+        <v>2</v>
+      </c>
+      <c r="E25" t="s">
+        <v>2</v>
+      </c>
+      <c r="F25" t="s">
+        <v>2</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1</v>
+      </c>
+      <c r="H25" t="s">
+        <v>2</v>
+      </c>
+      <c r="I25" t="s">
+        <v>2</v>
+      </c>
+      <c r="J25" t="s">
+        <v>1</v>
+      </c>
+      <c r="K25" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Team Attendence -  31-08 and 29-08
Team Attendence -  31-08 and 29-08
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CODE-MIND\Angular\JS-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D5C245A5-B75E-4B8E-B432-F9F51A168609}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCA78DB-CE3A-4646-AE61-94C236DCBB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1402,12 +1402,156 @@
         </r>
       </text>
     </comment>
+    <comment ref="C26" authorId="0" shapeId="0" xr:uid="{2D68FD1F-36EB-41B2-811C-8CFF71AE2967}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Health Issue</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G26" authorId="0" shapeId="0" xr:uid="{9E532A51-9170-4D5A-B6CA-7DAFBC114846}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F27" authorId="0" shapeId="0" xr:uid="{02CFEDD2-02CC-4D97-8FD0-9511770E1478}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Imegency</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G27" authorId="0" shapeId="0" xr:uid="{CE7B2DB9-7CB4-4AAE-9A69-AD9E4AF22D90}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H27" authorId="0" shapeId="0" xr:uid="{DEB7EC2F-2912-4033-8518-E3E616F52FA9}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Work in college</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I27" authorId="0" shapeId="0" xr:uid="{EF1568D1-6552-47D7-B605-B2374DF5F3C6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Outside</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="13">
   <si>
     <t>Date</t>
   </si>
@@ -1854,11 +1998,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L25"/>
+  <dimension ref="A1:L27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K25" sqref="K25"/>
+      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2542,6 +2686,76 @@
         <v>2</v>
       </c>
     </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A26" s="4">
+        <v>45166</v>
+      </c>
+      <c r="B26" t="s">
+        <v>2</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1</v>
+      </c>
+      <c r="D26" t="s">
+        <v>2</v>
+      </c>
+      <c r="E26" t="s">
+        <v>2</v>
+      </c>
+      <c r="F26" t="s">
+        <v>2</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1</v>
+      </c>
+      <c r="H26" t="s">
+        <v>2</v>
+      </c>
+      <c r="I26" t="s">
+        <v>2</v>
+      </c>
+      <c r="J26" t="s">
+        <v>2</v>
+      </c>
+      <c r="K26" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>45167</v>
+      </c>
+      <c r="B27" t="s">
+        <v>2</v>
+      </c>
+      <c r="C27" t="s">
+        <v>2</v>
+      </c>
+      <c r="D27" t="s">
+        <v>2</v>
+      </c>
+      <c r="E27" t="s">
+        <v>2</v>
+      </c>
+      <c r="F27" t="s">
+        <v>1</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1</v>
+      </c>
+      <c r="H27" t="s">
+        <v>1</v>
+      </c>
+      <c r="I27" t="s">
+        <v>1</v>
+      </c>
+      <c r="J27" t="s">
+        <v>2</v>
+      </c>
+      <c r="K27" t="s">
+        <v>2</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
B8-B1=Team Attendance - 05-Sep-23
B8-B1=Team Attendance - 05-Sep-23
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CODE-MIND\Angular\JS-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BCA78DB-CE3A-4646-AE61-94C236DCBB38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C125DC-A046-4C45-A61B-B1D4F82879A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1546,12 +1546,156 @@
         </r>
       </text>
     </comment>
+    <comment ref="G30" authorId="0" shapeId="0" xr:uid="{5FC65342-C605-41FB-B83F-6C08854799A1}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I30" authorId="0" shapeId="0" xr:uid="{D2ED0A9A-A95F-4CEA-9D9A-9170F98318C2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J30" authorId="0" shapeId="0" xr:uid="{230B252A-071E-4318-9186-72BB2C7B75F3}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K30" authorId="0" shapeId="0" xr:uid="{5558460E-9A3A-4537-9C0F-9D7109646597}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No Response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G31" authorId="0" shapeId="0" xr:uid="{49D680CA-8309-4F37-84E5-A67C4C506F40}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No response</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K31" authorId="0" shapeId="0" xr:uid="{D2E5B5A0-9942-447B-A0CC-3E6DABAB4787}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+No response</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="211" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -1590,6 +1734,9 @@
   </si>
   <si>
     <t>RaviKumar S</t>
+  </si>
+  <si>
+    <t>No Meeting</t>
   </si>
 </sst>
 </file>
@@ -1998,11 +2145,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L27"/>
+  <dimension ref="A1:L31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A17" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F31" sqref="F31"/>
+      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2756,6 +2903,116 @@
         <v>2</v>
       </c>
     </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" s="4">
+        <v>45169</v>
+      </c>
+      <c r="B29" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" t="s">
+        <v>2</v>
+      </c>
+      <c r="D29" t="s">
+        <v>2</v>
+      </c>
+      <c r="E29" t="s">
+        <v>2</v>
+      </c>
+      <c r="F29" t="s">
+        <v>1</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" t="s">
+        <v>1</v>
+      </c>
+      <c r="I29" t="s">
+        <v>1</v>
+      </c>
+      <c r="J29" t="s">
+        <v>1</v>
+      </c>
+      <c r="K29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A30" s="4">
+        <v>45173</v>
+      </c>
+      <c r="B30" t="s">
+        <v>2</v>
+      </c>
+      <c r="C30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D30" t="s">
+        <v>2</v>
+      </c>
+      <c r="E30" t="s">
+        <v>2</v>
+      </c>
+      <c r="F30" t="s">
+        <v>2</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1</v>
+      </c>
+      <c r="H30" t="s">
+        <v>1</v>
+      </c>
+      <c r="I30" t="s">
+        <v>1</v>
+      </c>
+      <c r="J30" t="s">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" s="4">
+        <v>45174</v>
+      </c>
+      <c r="B31" t="s">
+        <v>2</v>
+      </c>
+      <c r="C31" t="s">
+        <v>2</v>
+      </c>
+      <c r="D31" t="s">
+        <v>2</v>
+      </c>
+      <c r="E31" t="s">
+        <v>2</v>
+      </c>
+      <c r="F31" t="s">
+        <v>2</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1</v>
+      </c>
+      <c r="H31" t="s">
+        <v>2</v>
+      </c>
+      <c r="I31" t="s">
+        <v>1</v>
+      </c>
+      <c r="J31" t="s">
+        <v>2</v>
+      </c>
+      <c r="K31" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
B8-B1 Team Attendance 06-09-23
B8-B1 Team Attendance 06-09-23
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CODE-MIND\Angular\JS-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9C125DC-A046-4C45-A61B-B1D4F82879A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43D2C2A-95DB-4AE9-A345-E1B2D83CF5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1695,7 +1695,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -2145,11 +2145,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L31"/>
+  <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H31" sqref="H31"/>
+      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3013,6 +3013,41 @@
         <v>1</v>
       </c>
     </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A32" s="4">
+        <v>45175</v>
+      </c>
+      <c r="B32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C32" t="s">
+        <v>2</v>
+      </c>
+      <c r="D32" t="s">
+        <v>2</v>
+      </c>
+      <c r="E32" t="s">
+        <v>2</v>
+      </c>
+      <c r="F32" t="s">
+        <v>2</v>
+      </c>
+      <c r="G32" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32" t="s">
+        <v>1</v>
+      </c>
+      <c r="I32" t="s">
+        <v>1</v>
+      </c>
+      <c r="J32" t="s">
+        <v>1</v>
+      </c>
+      <c r="K32" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
Team Attendance b8-B1 - 09/09/23
Team Attendance b8-B1 - 09/09/23
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CODE-MIND\Angular\JS-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43D2C2A-95DB-4AE9-A345-E1B2D83CF5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908B6E6F-6DCE-4ECA-8226-C3868CBB951D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1690,12 +1690,148 @@
         </r>
       </text>
     </comment>
+    <comment ref="G33" authorId="0" shapeId="0" xr:uid="{4C1D8D43-7116-41CA-BF31-D0EE762A3528}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+no reponse</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I33" authorId="0" shapeId="0" xr:uid="{9206B2F7-09CE-4819-965C-1E43F086F82A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+out of town
+</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C34" authorId="0" shapeId="0" xr:uid="{E2D6EA80-939B-49D3-9870-0701ED962DFE}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:
+outide</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H34" authorId="0" shapeId="0" xr:uid="{E3C21121-43DE-4AC7-94B1-57CCB09C2AA6}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+outsside</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="J34" authorId="0" shapeId="0" xr:uid="{C0C54C8B-82A0-422E-B46D-55F38449F04C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Stuck in rain</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="K34" authorId="0" shapeId="0" xr:uid="{814A2A9A-286D-4A9A-A11D-07B197E9C3EB}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>LENOVO:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Some work</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -2145,11 +2281,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K32" sqref="K32"/>
+      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3048,6 +3184,111 @@
         <v>1</v>
       </c>
     </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A33" s="4">
+        <v>45176</v>
+      </c>
+      <c r="B33" t="s">
+        <v>2</v>
+      </c>
+      <c r="C33" t="s">
+        <v>2</v>
+      </c>
+      <c r="D33" t="s">
+        <v>2</v>
+      </c>
+      <c r="E33" t="s">
+        <v>2</v>
+      </c>
+      <c r="F33" t="s">
+        <v>2</v>
+      </c>
+      <c r="G33" t="s">
+        <v>1</v>
+      </c>
+      <c r="H33" t="s">
+        <v>1</v>
+      </c>
+      <c r="I33" t="s">
+        <v>1</v>
+      </c>
+      <c r="J33" t="s">
+        <v>2</v>
+      </c>
+      <c r="K33" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A34" s="4">
+        <v>45177</v>
+      </c>
+      <c r="B34" t="s">
+        <v>2</v>
+      </c>
+      <c r="C34" t="s">
+        <v>1</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34" t="s">
+        <v>2</v>
+      </c>
+      <c r="F34" t="s">
+        <v>2</v>
+      </c>
+      <c r="G34" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34" t="s">
+        <v>1</v>
+      </c>
+      <c r="I34" t="s">
+        <v>1</v>
+      </c>
+      <c r="J34" t="s">
+        <v>1</v>
+      </c>
+      <c r="K34" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" s="4">
+        <v>45178</v>
+      </c>
+      <c r="B35" t="s">
+        <v>2</v>
+      </c>
+      <c r="C35" t="s">
+        <v>2</v>
+      </c>
+      <c r="D35" t="s">
+        <v>2</v>
+      </c>
+      <c r="E35" t="s">
+        <v>2</v>
+      </c>
+      <c r="F35" t="s">
+        <v>2</v>
+      </c>
+      <c r="G35" t="s">
+        <v>1</v>
+      </c>
+      <c r="H35" t="s">
+        <v>1</v>
+      </c>
+      <c r="I35" t="s">
+        <v>1</v>
+      </c>
+      <c r="J35" t="s">
+        <v>2</v>
+      </c>
+      <c r="K35" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>

<commit_message>
TEAM ATTENDANCE B8-B1 12/09/23
TEAM ATTENDANCE B8-B1 12/09/23
</commit_message>
<xml_diff>
--- a/Team_Everyday_Attendence.xlsx
+++ b/Team_Everyday_Attendence.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="I:\CODE-MIND\Angular\JS-learning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{908B6E6F-6DCE-4ECA-8226-C3868CBB951D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BD27132-CD01-4172-8E42-5406A6AD62B1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{B014E2FF-8A25-5D4B-81D2-BF942392318A}"/>
   </bookViews>
@@ -1831,7 +1831,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="14">
   <si>
     <t>Date</t>
   </si>
@@ -2281,11 +2281,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6E3B6599-6209-4249-B0C6-73BAEC4B8C71}">
-  <dimension ref="A1:L35"/>
+  <dimension ref="A1:L37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K35" sqref="K35"/>
+      <selection pane="bottomLeft" activeCell="K37" sqref="K37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3289,6 +3289,76 @@
         <v>1</v>
       </c>
     </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" s="4">
+        <v>45180</v>
+      </c>
+      <c r="B36" t="s">
+        <v>2</v>
+      </c>
+      <c r="C36" t="s">
+        <v>2</v>
+      </c>
+      <c r="D36" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" t="s">
+        <v>2</v>
+      </c>
+      <c r="G36" t="s">
+        <v>1</v>
+      </c>
+      <c r="H36" t="s">
+        <v>1</v>
+      </c>
+      <c r="I36" t="s">
+        <v>2</v>
+      </c>
+      <c r="J36" t="s">
+        <v>1</v>
+      </c>
+      <c r="K36" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" s="4">
+        <v>45181</v>
+      </c>
+      <c r="B37" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D37" t="s">
+        <v>2</v>
+      </c>
+      <c r="E37" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" t="s">
+        <v>2</v>
+      </c>
+      <c r="G37" t="s">
+        <v>2</v>
+      </c>
+      <c r="H37" t="s">
+        <v>1</v>
+      </c>
+      <c r="I37" t="s">
+        <v>2</v>
+      </c>
+      <c r="J37" t="s">
+        <v>2</v>
+      </c>
+      <c r="K37" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <dataValidations count="2">

</xml_diff>